<commit_message>
update add resto + credit
</commit_message>
<xml_diff>
--- a/public/resto.xlsx
+++ b/public/resto.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.truong\OneDrive - LPA-LyonParcAuto\Documents\GitHub\RestoRoulette\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76EE3FBC-CBD6-41A7-BCB1-6A7FEB5A2169}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FF468A4-3D1F-4577-9C00-582082FFCD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8A0F603C-F464-4664-BB50-D3DFE8858AF2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t>lat</t>
   </si>
@@ -113,9 +113,6 @@
     <t>nom</t>
   </si>
   <si>
-    <t>https://lh3.googleusercontent.com/gps-cs-s/AC9h4nppPrgF4SIF9TKpmouifNx3mEKp6LYUhudkDD4_s_ftPlYGcmDdjSLWeEJdIQfzgSCRHD72w9QQxuqJjnwbTtCB6gWodXzqjkN8mp53qK4W9LCzIkrj5tF_tFpmNCjtbaCuGmJMKUJ3hCf0=s1360-w1360-h1020</t>
-  </si>
-  <si>
     <t>image</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>https://www.lyoncapitale.fr/wp-content/uploads/2024/07/IMG_9609-e1720593864506.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">https://lh3.googleusercontent.com/gps-cs-s/AC9h4np9QK393ruj1nrQb6x392Q4hT8EYc65sFA94ccukxDmxHBdHNdzcjWBj_kJqCi8WRDwO9pg26gDLnDPOUNa19zVKb2m39A4fxieKfQdAz3hmMeAQWq26utRRT0lcIYJapyFrm0E=s1360-w1360-h1020 </t>
-  </si>
-  <si>
     <t xml:space="preserve">https://i0.wp.com/lyon.citycrunch.fr/wp-content/uploads/sites/3/2021/06/banneton_Lyon-CityCrunch-4.jpg?resize=800%2C800&amp;ssl=1 </t>
   </si>
   <si>
@@ -261,6 +255,36 @@
   </si>
   <si>
     <t>4.835084823452183</t>
+  </si>
+  <si>
+    <t>https://dalilk-europe.com/wp-content/uploads/2022/04/Le-Roi-Falafel-1.jpg</t>
+  </si>
+  <si>
+    <t>https://dynamic-media-cdn.tripadvisor.com/media/photo-o/21/d0/08/f6/ben-s-bowl.jpg?w=1000&amp;h=-1&amp;s=1</t>
+  </si>
+  <si>
+    <t>https://i0.wp.com/lyon.citycrunch.fr/wp-content/uploads/sites/3/2019/11/bouillon-maurice-Lyoncitycrunch-5.jpg?resize=800%2C800&amp;ssl=1</t>
+  </si>
+  <si>
+    <t>4.835304</t>
+  </si>
+  <si>
+    <t>45.763044</t>
+  </si>
+  <si>
+    <t>Bouillon Maurice</t>
+  </si>
+  <si>
+    <t>L'Entrecôte</t>
+  </si>
+  <si>
+    <t>45.765579</t>
+  </si>
+  <si>
+    <t>4.835788</t>
+  </si>
+  <si>
+    <t>https://voiretmanger.fr/wp-content/uploads/2011/10/l_entrecote-lyon.jpg</t>
   </si>
 </sst>
 </file>
@@ -335,7 +359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -355,6 +379,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -365,10 +392,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -399,18 +426,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28E6809D-4C59-4EB8-BAF3-F1C134175E04}" name="Tableau1" displayName="Tableau1" ref="A1:F13" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F13" xr:uid="{28E6809D-4C59-4EB8-BAF3-F1C134175E04}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28E6809D-4C59-4EB8-BAF3-F1C134175E04}" name="Tableau1" displayName="Tableau1" ref="A1:F15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F15" xr:uid="{28E6809D-4C59-4EB8-BAF3-F1C134175E04}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D9">
     <sortCondition ref="A1:A9"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{D61BBC64-E82B-49EF-B324-E981E4723188}" name="nom" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{D9D6F0A2-5BE8-46CA-A163-67F5C6E5ACDF}" name="lat" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{C484BB70-22AB-4362-9BF8-EEF08C60D5A9}" name="lon" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{8DE441C8-7D94-495A-B55F-680F4239A247}" name="image" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{22A07948-A0FB-4136-81A4-7F6FC7321DE7}" name="menu" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{C4FED95E-8485-4CDE-929C-525D49D2EA43}" name="menu_image" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D61BBC64-E82B-49EF-B324-E981E4723188}" name="nom" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{D9D6F0A2-5BE8-46CA-A163-67F5C6E5ACDF}" name="lat" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{C484BB70-22AB-4362-9BF8-EEF08C60D5A9}" name="lon" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{8DE441C8-7D94-495A-B55F-680F4239A247}" name="image" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{22A07948-A0FB-4136-81A4-7F6FC7321DE7}" name="menu" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C4FED95E-8485-4CDE-929C-525D49D2EA43}" name="menu_image" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -734,16 +761,17 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61EBC5B-CD90-426E-8B1B-BC086E254604}">
   <sheetPr codeName="Feuil1"/>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="21.7109375" customWidth="1"/>
+    <col min="2" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -757,13 +785,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -777,13 +805,13 @@
         <v>14</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -797,18 +825,18 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>10</v>
@@ -817,13 +845,13 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -837,13 +865,13 @@
         <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -857,18 +885,18 @@
         <v>17</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -877,13 +905,13 @@
         <v>9</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -897,13 +925,13 @@
         <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -917,88 +945,120 @@
         <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="D10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>31</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="E12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C13" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1023,10 +1083,13 @@
     <hyperlink ref="E12" r:id="rId19" xr:uid="{8F4F116E-F1A3-4DD5-AA92-BB5B0A21BE29}"/>
     <hyperlink ref="D12" r:id="rId20" xr:uid="{0E7AB76B-A14F-43E7-B258-B21E3AA6A083}"/>
     <hyperlink ref="D13" r:id="rId21" xr:uid="{6C79BD45-DBAB-497E-B6A5-1BBDE078B666}"/>
+    <hyperlink ref="D14" r:id="rId22" xr:uid="{E4389ECE-580C-44C1-AB4B-000911F8B486}"/>
+    <hyperlink ref="D15" r:id="rId23" xr:uid="{FCA669D0-0DEE-4259-8479-3FE6A67995FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId24"/>
   <tableParts count="1">
-    <tablePart r:id="rId22"/>
+    <tablePart r:id="rId25"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>